<commit_message>
save 18 01 2026
</commit_message>
<xml_diff>
--- a/4 четверть_5_JavaScript_Front_события_медиафайлы.xlsx
+++ b/4 четверть_5_JavaScript_Front_события_медиафайлы.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Machenike\Desktop\Homework_repo\GB_Developer_Workbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Machenike\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89626132-C9E6-48FC-9DEA-8E4C2773BF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500E58A5-4CA0-496A-8F6B-AB65189CE226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{D02F8FAA-6DBD-4917-AAE5-BA1803CF7D1E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="624">
   <si>
     <t>Мышка</t>
   </si>
@@ -6661,12 +6661,552 @@
     <t xml:space="preserve">
 </t>
   </si>
+  <si>
+    <t>Преимущества кастомных событий</t>
+  </si>
+  <si>
+    <t>легко менять триггеры без переписывания реакций;</t>
+  </si>
+  <si>
+    <t>Делают код гибким</t>
+  </si>
+  <si>
+    <t>Передача данных между компонентами или частями приложения</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Пояснение! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Стандартные события (click, change) не позволяют легко передавать произвольные данные, а CustomEvent — да, через свойство detail.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const customEvent = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>new CustomEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>('</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>userLoggedIn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">', {
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>detail: { userId: 123, name: 'Анна' }</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+});
+window.dispatchEvent(customEvent);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>window.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>addEventListener</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>('</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>userLoggedIn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>', (event) =&gt; {
+  console.log(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>event.detail.name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>); // → "Анна"
+});</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Где-то в другом месте
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Пояснение! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Они не знают друг о друге напрямую — связь идёт через DOM или EventBus.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Еще вариант - прямой вызов нового события!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+element.dispatchEvent(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>new CustomEvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>('</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>themeChanged</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>', { detail: { theme: 'dark' } }));</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>function closeModal(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>modalId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) {
+  // ... закрываем модалку с ID modalId
+  const event = new CustomEvent('modalClosed', {
+    bubbles: true,
+    detail: { </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>modalId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> }
+  });
+  document.dispatchEvent(event);
+}
+// Где-то в коде:
+closeModal(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'cart-modal'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);     // → вызовет updateCart()
+closeModal(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'checkout-modal'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>); // → вызовет checkoutModal()</t>
+    </r>
+  </si>
+  <si>
+    <t>window.addEventListener('modalClosed', (event) =&gt; {
+  if (event.detail.modalId === 'cart-modal') updateCart();
+  if (event.detail.modalId === 'checkout-modal') checkoutModal();
+});</t>
+  </si>
+  <si>
+    <t>аналог EventBus</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Пояснение!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Возможность не перегружать логику одного встроенного события, например click, делая возможным не дублировать кода при вызове того же события через клавишу Esc, … или другой вызов события click</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Важно!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bubbles: true
+Поскольку событие отправляется через document, всплытие не критично, но если вы будете диспетчеризировать событие на элементе (например, modalElement.dispatchEvent(...)), то bubbles: true позволит поймать его на document.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Важно!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Если вы добавляете слушатели динамически (например, в компонентах), не забывайте их удалять, чтобы избежать утечек памяти.</t>
+    </r>
+  </si>
+  <si>
+    <t>Без использования кастомных событий, если изменение нужно сделать в одном модуле</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">unction closeModal(modalId, onClose) {
+  // ... закрыть модальное окно
+  onClose?.(modalId);
+}
+closeModal('cart-modal', (id) =&gt; {
+  if (id === 'cart-modal') updateCart();
+});
+// В корзине:
+closeModal('cart-modal', () =&gt; updateCart());
+// В аналитике:
+closeModal('promo-modal', () =&gt; sendAnalytics('promo_closed'));
+// Без побочных эффектов:
+closeModal('info-modal'); // onClose не передан → ничего не происходит
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Почему такое написание лучше!
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>closeModal — это UI-логика (работа с модальными окнами).
+updateCart() — это бизнес-логика (работа с данными корзины).</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6767,6 +7307,15 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -6882,7 +7431,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -7107,6 +7656,9 @@
     <xf numFmtId="49" fontId="11" fillId="15" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -7135,13 +7687,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>41919</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2184638</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>1359051</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7615,10 +8167,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7742,7 +8294,7 @@
       <c r="B10" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="80" t="s">
         <v>588</v>
       </c>
       <c r="D10" s="15" t="s">
@@ -7754,87 +8306,161 @@
       <c r="B11" s="15" t="s">
         <v>590</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="80" t="s">
         <v>591</v>
       </c>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
-        <v>606</v>
-      </c>
-      <c r="B12" s="15"/>
+        <v>608</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>619</v>
+      </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:22" ht="116" x14ac:dyDescent="0.35">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15" t="s">
-        <v>607</v>
-      </c>
+    <row r="13" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="77" t="s">
+        <v>611</v>
+      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
+      <c r="B14" s="80" t="s">
+        <v>612</v>
+      </c>
+      <c r="C14" s="80" t="s">
+        <v>613</v>
+      </c>
+      <c r="D14" s="80" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="15"/>
+      <c r="B15" s="80" t="s">
+        <v>615</v>
+      </c>
+      <c r="C15" s="80" t="s">
+        <v>614</v>
+      </c>
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="77" t="s">
+        <v>610</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15" t="s">
+        <v>609</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="15"/>
+      <c r="B17" s="80" t="s">
+        <v>620</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="15"/>
+      <c r="B18" s="80" t="s">
+        <v>621</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>618</v>
+      </c>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
+        <v>606</v>
+      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" ht="116" x14ac:dyDescent="0.35">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15" t="s">
+        <v>607</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="16" t="s">
         <v>592</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:22" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
         <v>593</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B22" s="15" t="s">
         <v>594</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C22" s="15" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="C16" s="15" t="s">
+    <row r="23" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="C23" s="15" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="B17" s="15" t="s">
+    <row r="24" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="15" t="s">
         <v>597</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C24" s="15" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="16" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="16" t="s">
         <v>599</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="C19" s="15" t="s">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+    </row>
+    <row r="26" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="C26" s="15" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="145" x14ac:dyDescent="0.35">
-      <c r="B20" s="15" t="s">
+    <row r="27" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="B27" s="15" t="s">
         <v>601</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C27" s="15" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="145" x14ac:dyDescent="0.35">
-      <c r="B21" s="78" t="s">
+    <row r="28" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+      <c r="B28" s="78" t="s">
         <v>603</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C28" s="15" t="s">
         <v>604</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>605</v>
       </c>
     </row>

</xml_diff>